<commit_message>
This is updated working with Rule ID
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/rules.xlsx
+++ b/src/main/resources/rules/rules.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>RuleSet</t>
   </si>
@@ -90,10 +90,10 @@
     <t>Diamond#4</t>
   </si>
   <si>
-    <t>Diamond#5</t>
-  </si>
-  <si>
-    <t>nz</t>
+    <t>$productObject.setRule($param);</t>
+  </si>
+  <si>
+    <t>RuleID</t>
   </si>
 </sst>
 </file>
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -224,9 +224,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -251,32 +248,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,7 +659,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -707,7 +701,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -727,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -739,22 +733,23 @@
     <col min="2" max="2" width="35.88671875" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" outlineLevel="1">
+    <row r="1" spans="1:6" outlineLevel="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:9" ht="38.1" customHeight="1" outlineLevel="1">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:6" ht="38.1" customHeight="1" outlineLevel="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -763,34 +758,32 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="1:9" outlineLevel="1">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" outlineLevel="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" outlineLevel="1">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" outlineLevel="1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -803,137 +796,139 @@
       <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" outlineLevel="1">
-      <c r="B7" s="21" t="s">
+      <c r="F6" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" outlineLevel="1">
+      <c r="B7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="6"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="26.4" outlineLevel="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="26.4" outlineLevel="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" outlineLevel="1">
-      <c r="A9" s="7" t="s">
+      <c r="F8" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" outlineLevel="1">
+      <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" outlineLevel="1">
-      <c r="A10" s="12" t="s">
+      <c r="F9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" outlineLevel="1">
+      <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="8">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="12" t="s">
+      <c r="F10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="8">
+      <c r="D11" s="10"/>
+      <c r="E11" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="12" t="s">
+      <c r="F11" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="12" t="s">
+      <c r="F12" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="E13" s="7">
         <v>25</v>
       </c>
-      <c r="E14" s="8">
-        <v>35</v>
+      <c r="F13" s="14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="3">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B1:E1"/>
+  <mergeCells count="2">
     <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
This is testing branch
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/rules.xlsx
+++ b/src/main/resources/rules/rules.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>RuleSet</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>RuleID</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Diamond#5</t>
+  </si>
+  <si>
+    <t>Diamond#6</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -260,6 +272,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,9 +283,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,7 +671,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -701,7 +713,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -721,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -732,24 +744,25 @@
     <col min="1" max="1" width="32.88671875" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="4" max="5" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" outlineLevel="1">
+    <row r="1" spans="1:7" outlineLevel="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="38.1" customHeight="1" outlineLevel="1">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" ht="38.1" customHeight="1" outlineLevel="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -760,8 +773,9 @@
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" outlineLevel="1">
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" outlineLevel="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -772,8 +786,9 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -782,8 +797,9 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" outlineLevel="1">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" outlineLevel="1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -796,23 +812,27 @@
       <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>4</v>
+      <c r="E6" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" outlineLevel="1">
-      <c r="B7" s="18" t="s">
+      <c r="G6" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" outlineLevel="1">
+      <c r="B7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="20"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="26.4" outlineLevel="1">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="26.4" outlineLevel="1">
       <c r="A8" s="9"/>
       <c r="B8" s="12" t="s">
         <v>10</v>
@@ -823,14 +843,17 @@
       <c r="D8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" outlineLevel="1">
+    <row r="9" spans="1:7" outlineLevel="1">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -844,13 +867,16 @@
         <v>13</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" outlineLevel="1">
+    <row r="10" spans="1:7" outlineLevel="1">
       <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
@@ -859,14 +885,15 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="7">
+      <c r="E10" s="10"/>
+      <c r="F10" s="7">
         <v>15</v>
       </c>
-      <c r="F10" s="14">
+      <c r="G10" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -877,14 +904,15 @@
         <v>17</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="7">
+      <c r="E11" s="10"/>
+      <c r="F11" s="7">
         <v>20</v>
       </c>
-      <c r="F11" s="14">
+      <c r="G11" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -897,14 +925,17 @@
       <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="7">
-        <v>25</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="E12" s="10">
+        <v>100</v>
+      </c>
+      <c r="F12" s="7">
+        <v>30</v>
+      </c>
+      <c r="G12" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="11" t="s">
         <v>23</v>
       </c>
@@ -915,20 +946,69 @@
         <v>17</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="10">
+        <v>100</v>
+      </c>
+      <c r="F13" s="7">
+        <v>35</v>
+      </c>
+      <c r="G13" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="7">
-        <v>25</v>
-      </c>
-      <c r="F13" s="14">
-        <v>4</v>
+      <c r="E14" s="10">
+        <v>500</v>
+      </c>
+      <c r="F14" s="7">
+        <v>17</v>
+      </c>
+      <c r="G14" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="10">
+        <v>100</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="2">
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>